<commit_message>
[feat] added some shit
</commit_message>
<xml_diff>
--- a/orders.xlsx
+++ b/orders.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Orders" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Orders" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,17 +444,64 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
+          <t>orders_count</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
           <t>check_link</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>timestamp</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>username</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>0000001</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>test, test, test</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>https://gift-bot-checks.s3.us-east-1.amazonaws.com/checks/AQADFOgxG3JVYEt-.jpg</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>2024-12-25 22:28:44</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>wakeupkstnv</t>
         </is>
       </c>
     </row>

</xml_diff>